<commit_message>
Se depura reloj matriz 16x16
</commit_message>
<xml_diff>
--- a/DOCS/Digitos_5x8.xlsx
+++ b/DOCS/Digitos_5x8.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="2">
   <si>
     <t xml:space="preserve">n</t>
   </si>
@@ -199,10 +199,10 @@
   <dimension ref="A1:AD997"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A65" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A79" activeCellId="0" sqref="A79"/>
+      <selection pane="topLeft" activeCell="A79" activeCellId="1" sqref="N2:N87 A79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="0" width="3.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9"/>
@@ -19431,10 +19431,10 @@
   <dimension ref="A1:L87"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B82" activeCellId="0" sqref="B82"/>
+      <selection pane="topLeft" activeCell="B82" activeCellId="1" sqref="N2:N87 B82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="0" width="4.02"/>
@@ -21890,10 +21890,10 @@
   <dimension ref="A1:L65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B62" activeCellId="0" sqref="B62"/>
+      <selection pane="topLeft" activeCell="B62" activeCellId="1" sqref="N2:N87 B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="4.02"/>
@@ -23531,13 +23531,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L87"/>
+  <dimension ref="A1:N87"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F42" activeCellId="0" sqref="F42"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A56" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2:N87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="0" width="4.02"/>
@@ -23605,6 +23605,14 @@
         <f aca="false">CONCATENATE("&amp;B",J2)</f>
         <v>&amp;B00111110</v>
       </c>
+      <c r="M2" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B2="n","1","0"),IF(C2="n","1","0"),IF(D2="n","1","0"),IF(E2="n","1","0"),IF(F2="n","1","0"),IF(G2="n","1","0"),IF(H2="n","1","0"),IF(I2="n","1","0"))</f>
+        <v>01111100</v>
+      </c>
+      <c r="N2" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M2,",")</f>
+        <v>0B01111100,</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
@@ -23642,6 +23650,14 @@
       <c r="L3" s="1" t="str">
         <f aca="false">CONCATENATE("&amp;B",J3)</f>
         <v>&amp;B01111111</v>
+      </c>
+      <c r="M3" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B3="n","1","0"),IF(C3="n","1","0"),IF(D3="n","1","0"),IF(E3="n","1","0"),IF(F3="n","1","0"),IF(G3="n","1","0"),IF(H3="n","1","0"),IF(I3="n","1","0"))</f>
+        <v>11111110</v>
+      </c>
+      <c r="N3" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M3,",")</f>
+        <v>0B11111110,</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23671,6 +23687,14 @@
         <f aca="false">CONCATENATE("&amp;B",J4)</f>
         <v>&amp;B01000001</v>
       </c>
+      <c r="M4" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B4="n","1","0"),IF(C4="n","1","0"),IF(D4="n","1","0"),IF(E4="n","1","0"),IF(F4="n","1","0"),IF(G4="n","1","0"),IF(H4="n","1","0"),IF(I4="n","1","0"))</f>
+        <v>10000010</v>
+      </c>
+      <c r="N4" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M4,",")</f>
+        <v>0B10000010,</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
@@ -23699,6 +23723,14 @@
         <f aca="false">CONCATENATE("&amp;B",J5)</f>
         <v>&amp;B01000001</v>
       </c>
+      <c r="M5" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B5="n","1","0"),IF(C5="n","1","0"),IF(D5="n","1","0"),IF(E5="n","1","0"),IF(F5="n","1","0"),IF(G5="n","1","0"),IF(H5="n","1","0"),IF(I5="n","1","0"))</f>
+        <v>10000010</v>
+      </c>
+      <c r="N5" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M5,",")</f>
+        <v>0B10000010,</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
@@ -23736,6 +23768,14 @@
       <c r="L6" s="1" t="str">
         <f aca="false">CONCATENATE("&amp;B",J6)</f>
         <v>&amp;B01111111</v>
+      </c>
+      <c r="M6" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B6="n","1","0"),IF(C6="n","1","0"),IF(D6="n","1","0"),IF(E6="n","1","0"),IF(F6="n","1","0"),IF(G6="n","1","0"),IF(H6="n","1","0"),IF(I6="n","1","0"))</f>
+        <v>11111110</v>
+      </c>
+      <c r="N6" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M6,",")</f>
+        <v>0B11111110,</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23771,6 +23811,17 @@
         <f aca="false">CONCATENATE("&amp;B",J7)</f>
         <v>&amp;B00111110</v>
       </c>
+      <c r="M7" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B7="n","1","0"),IF(C7="n","1","0"),IF(D7="n","1","0"),IF(E7="n","1","0"),IF(F7="n","1","0"),IF(G7="n","1","0"),IF(H7="n","1","0"),IF(I7="n","1","0"))</f>
+        <v>01111100</v>
+      </c>
+      <c r="N7" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M7,",")</f>
+        <v>0B01111100,</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="n">
@@ -23800,6 +23851,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
@@ -23824,6 +23876,14 @@
         <f aca="false">CONCATENATE("&amp;B",J10)</f>
         <v>&amp;B00000000</v>
       </c>
+      <c r="M10" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B10="n","1","0"),IF(C10="n","1","0"),IF(D10="n","1","0"),IF(E10="n","1","0"),IF(F10="n","1","0"),IF(G10="n","1","0"),IF(H10="n","1","0"),IF(I10="n","1","0"))</f>
+        <v>00000000</v>
+      </c>
+      <c r="N10" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M10,",")</f>
+        <v>0B00000000,</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
@@ -23852,6 +23912,14 @@
         <f aca="false">CONCATENATE("&amp;B",J11)</f>
         <v>&amp;B00100001</v>
       </c>
+      <c r="M11" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B11="n","1","0"),IF(C11="n","1","0"),IF(D11="n","1","0"),IF(E11="n","1","0"),IF(F11="n","1","0"),IF(G11="n","1","0"),IF(H11="n","1","0"),IF(I11="n","1","0"))</f>
+        <v>10000100</v>
+      </c>
+      <c r="N11" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M11,",")</f>
+        <v>0B10000100,</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
@@ -23890,6 +23958,14 @@
         <f aca="false">CONCATENATE("&amp;B",J12)</f>
         <v>&amp;B01111111</v>
       </c>
+      <c r="M12" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B12="n","1","0"),IF(C12="n","1","0"),IF(D12="n","1","0"),IF(E12="n","1","0"),IF(F12="n","1","0"),IF(G12="n","1","0"),IF(H12="n","1","0"),IF(I12="n","1","0"))</f>
+        <v>11111110</v>
+      </c>
+      <c r="N12" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M12,",")</f>
+        <v>0B11111110,</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
@@ -23927,6 +24003,14 @@
       <c r="L13" s="1" t="str">
         <f aca="false">CONCATENATE("&amp;B",J13)</f>
         <v>&amp;B01111111</v>
+      </c>
+      <c r="M13" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B13="n","1","0"),IF(C13="n","1","0"),IF(D13="n","1","0"),IF(E13="n","1","0"),IF(F13="n","1","0"),IF(G13="n","1","0"),IF(H13="n","1","0"),IF(I13="n","1","0"))</f>
+        <v>11111110</v>
+      </c>
+      <c r="N13" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M13,",")</f>
+        <v>0B11111110,</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23953,6 +24037,14 @@
       <c r="L14" s="1" t="str">
         <f aca="false">CONCATENATE("&amp;B",J14)</f>
         <v>&amp;B00000001</v>
+      </c>
+      <c r="M14" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B14="n","1","0"),IF(C14="n","1","0"),IF(D14="n","1","0"),IF(E14="n","1","0"),IF(F14="n","1","0"),IF(G14="n","1","0"),IF(H14="n","1","0"),IF(I14="n","1","0"))</f>
+        <v>10000000</v>
+      </c>
+      <c r="N14" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M14,",")</f>
+        <v>0B10000000,</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23978,6 +24070,17 @@
         <f aca="false">CONCATENATE("&amp;B",J15)</f>
         <v>&amp;B00000000</v>
       </c>
+      <c r="M15" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B15="n","1","0"),IF(C15="n","1","0"),IF(D15="n","1","0"),IF(E15="n","1","0"),IF(F15="n","1","0"),IF(G15="n","1","0"),IF(H15="n","1","0"),IF(I15="n","1","0"))</f>
+        <v>00000000</v>
+      </c>
+      <c r="N15" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M15,",")</f>
+        <v>0B00000000,</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1" t="n">
@@ -24007,6 +24110,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="n">
@@ -24035,6 +24139,14 @@
         <f aca="false">CONCATENATE("&amp;B",J18)</f>
         <v>&amp;B00100001</v>
       </c>
+      <c r="M18" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B18="n","1","0"),IF(C18="n","1","0"),IF(D18="n","1","0"),IF(E18="n","1","0"),IF(F18="n","1","0"),IF(G18="n","1","0"),IF(H18="n","1","0"),IF(I18="n","1","0"))</f>
+        <v>10000100</v>
+      </c>
+      <c r="N18" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M18,",")</f>
+        <v>0B10000100,</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="n">
@@ -24049,23 +24161,29 @@
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="G19" s="5"/>
       <c r="H19" s="5" t="s">
         <v>0</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="1" t="str">
         <f aca="false">CONCATENATE(IF(I19="n","1","0"),IF(H19="n","1","0"),IF(G19="n","1","0"),IF(F19="n","1","0"),IF(E19="n","1","0"),IF(D19="n","1","0"),IF(C19="n","1","0"),IF(B19="n","1","0"))</f>
-        <v>01100011</v>
+        <v>01000011</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L19" s="1" t="str">
         <f aca="false">CONCATENATE("&amp;B",J19)</f>
-        <v>&amp;B01100011</v>
+        <v>&amp;B01000011</v>
+      </c>
+      <c r="M19" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B19="n","1","0"),IF(C19="n","1","0"),IF(D19="n","1","0"),IF(E19="n","1","0"),IF(F19="n","1","0"),IF(G19="n","1","0"),IF(H19="n","1","0"),IF(I19="n","1","0"))</f>
+        <v>11000010</v>
+      </c>
+      <c r="N19" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M19,",")</f>
+        <v>0B11000010,</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24099,6 +24217,14 @@
         <f aca="false">CONCATENATE("&amp;B",J20)</f>
         <v>&amp;B01000111</v>
       </c>
+      <c r="M20" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B20="n","1","0"),IF(C20="n","1","0"),IF(D20="n","1","0"),IF(E20="n","1","0"),IF(F20="n","1","0"),IF(G20="n","1","0"),IF(H20="n","1","0"),IF(I20="n","1","0"))</f>
+        <v>11100010</v>
+      </c>
+      <c r="N20" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M20,",")</f>
+        <v>0B11100010,</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="n">
@@ -24131,6 +24257,14 @@
         <f aca="false">CONCATENATE("&amp;B",J21)</f>
         <v>&amp;B01001101</v>
       </c>
+      <c r="M21" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B21="n","1","0"),IF(C21="n","1","0"),IF(D21="n","1","0"),IF(E21="n","1","0"),IF(F21="n","1","0"),IF(G21="n","1","0"),IF(H21="n","1","0"),IF(I21="n","1","0"))</f>
+        <v>10110010</v>
+      </c>
+      <c r="N21" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M21,",")</f>
+        <v>0B10110010,</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="n">
@@ -24164,6 +24298,14 @@
       <c r="L22" s="1" t="str">
         <f aca="false">CONCATENATE("&amp;B",J22)</f>
         <v>&amp;B01111001</v>
+      </c>
+      <c r="M22" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B22="n","1","0"),IF(C22="n","1","0"),IF(D22="n","1","0"),IF(E22="n","1","0"),IF(F22="n","1","0"),IF(G22="n","1","0"),IF(H22="n","1","0"),IF(I22="n","1","0"))</f>
+        <v>10011110</v>
+      </c>
+      <c r="N22" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M22,",")</f>
+        <v>0B10011110,</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24195,6 +24337,17 @@
         <f aca="false">CONCATENATE("&amp;B",J23)</f>
         <v>&amp;B00110001</v>
       </c>
+      <c r="M23" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B23="n","1","0"),IF(C23="n","1","0"),IF(D23="n","1","0"),IF(E23="n","1","0"),IF(F23="n","1","0"),IF(G23="n","1","0"),IF(H23="n","1","0"),IF(I23="n","1","0"))</f>
+        <v>10001100</v>
+      </c>
+      <c r="N23" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M23,",")</f>
+        <v>0B10001100,</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="n">
@@ -24224,33 +24377,42 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="B26" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="I26" s="5"/>
       <c r="J26" s="1" t="str">
         <f aca="false">CONCATENATE(IF(I26="n","1","0"),IF(H26="n","1","0"),IF(G26="n","1","0"),IF(F26="n","1","0"),IF(E26="n","1","0"),IF(D26="n","1","0"),IF(C26="n","1","0"),IF(B26="n","1","0"))</f>
-        <v>00100010</v>
+        <v>01000001</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L26" s="1" t="str">
         <f aca="false">CONCATENATE("&amp;B",J26)</f>
-        <v>&amp;B00100010</v>
+        <v>&amp;B01000001</v>
+      </c>
+      <c r="M26" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B26="n","1","0"),IF(C26="n","1","0"),IF(D26="n","1","0"),IF(E26="n","1","0"),IF(F26="n","1","0"),IF(G26="n","1","0"),IF(H26="n","1","0"),IF(I26="n","1","0"))</f>
+        <v>10000010</v>
+      </c>
+      <c r="N26" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M26,",")</f>
+        <v>0B10000010,</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24260,29 +24422,33 @@
       <c r="B27" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="G27" s="5"/>
       <c r="H27" s="5" t="s">
         <v>0</v>
       </c>
       <c r="I27" s="5"/>
       <c r="J27" s="1" t="str">
         <f aca="false">CONCATENATE(IF(I27="n","1","0"),IF(H27="n","1","0"),IF(G27="n","1","0"),IF(F27="n","1","0"),IF(E27="n","1","0"),IF(D27="n","1","0"),IF(C27="n","1","0"),IF(B27="n","1","0"))</f>
-        <v>01100011</v>
+        <v>01000001</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L27" s="1" t="str">
         <f aca="false">CONCATENATE("&amp;B",J27)</f>
-        <v>&amp;B01100011</v>
+        <v>&amp;B01000001</v>
+      </c>
+      <c r="M27" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B27="n","1","0"),IF(C27="n","1","0"),IF(D27="n","1","0"),IF(E27="n","1","0"),IF(F27="n","1","0"),IF(G27="n","1","0"),IF(H27="n","1","0"),IF(I27="n","1","0"))</f>
+        <v>10000010</v>
+      </c>
+      <c r="N27" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M27,",")</f>
+        <v>0B10000010,</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24314,6 +24480,14 @@
         <f aca="false">CONCATENATE("&amp;B",J28)</f>
         <v>&amp;B01001001</v>
       </c>
+      <c r="M28" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B28="n","1","0"),IF(C28="n","1","0"),IF(D28="n","1","0"),IF(E28="n","1","0"),IF(F28="n","1","0"),IF(G28="n","1","0"),IF(H28="n","1","0"),IF(I28="n","1","0"))</f>
+        <v>10010010</v>
+      </c>
+      <c r="N28" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M28,",")</f>
+        <v>0B10010010,</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="n">
@@ -24344,6 +24518,14 @@
         <f aca="false">CONCATENATE("&amp;B",J29)</f>
         <v>&amp;B01001001</v>
       </c>
+      <c r="M29" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B29="n","1","0"),IF(C29="n","1","0"),IF(D29="n","1","0"),IF(E29="n","1","0"),IF(F29="n","1","0"),IF(G29="n","1","0"),IF(H29="n","1","0"),IF(I29="n","1","0"))</f>
+        <v>10010010</v>
+      </c>
+      <c r="N29" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M29,",")</f>
+        <v>0B10010010,</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="n">
@@ -24381,6 +24563,14 @@
       <c r="L30" s="1" t="str">
         <f aca="false">CONCATENATE("&amp;B",J30)</f>
         <v>&amp;B01111111</v>
+      </c>
+      <c r="M30" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B30="n","1","0"),IF(C30="n","1","0"),IF(D30="n","1","0"),IF(E30="n","1","0"),IF(F30="n","1","0"),IF(G30="n","1","0"),IF(H30="n","1","0"),IF(I30="n","1","0"))</f>
+        <v>11111110</v>
+      </c>
+      <c r="N30" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M30,",")</f>
+        <v>0B11111110,</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24414,6 +24604,17 @@
         <f aca="false">CONCATENATE("&amp;B",J31)</f>
         <v>&amp;B00110110</v>
       </c>
+      <c r="M31" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B31="n","1","0"),IF(C31="n","1","0"),IF(D31="n","1","0"),IF(E31="n","1","0"),IF(F31="n","1","0"),IF(G31="n","1","0"),IF(H31="n","1","0"),IF(I31="n","1","0"))</f>
+        <v>01101100</v>
+      </c>
+      <c r="N31" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M31,",")</f>
+        <v>0B01101100,</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="n">
@@ -24443,6 +24644,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="n">
@@ -24459,19 +24661,29 @@
       <c r="F34" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G34" s="5"/>
+      <c r="G34" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
       <c r="J34" s="1" t="str">
         <f aca="false">CONCATENATE(IF(I34="n","1","0"),IF(H34="n","1","0"),IF(G34="n","1","0"),IF(F34="n","1","0"),IF(E34="n","1","0"),IF(D34="n","1","0"),IF(C34="n","1","0"),IF(B34="n","1","0"))</f>
-        <v>00011100</v>
+        <v>00111100</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L34" s="1" t="str">
         <f aca="false">CONCATENATE("&amp;B",J34)</f>
-        <v>&amp;B00011100</v>
+        <v>&amp;B00111100</v>
+      </c>
+      <c r="M34" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B34="n","1","0"),IF(C34="n","1","0"),IF(D34="n","1","0"),IF(E34="n","1","0"),IF(F34="n","1","0"),IF(G34="n","1","0"),IF(H34="n","1","0"),IF(I34="n","1","0"))</f>
+        <v>00111100</v>
+      </c>
+      <c r="N34" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M34,",")</f>
+        <v>0B00111100,</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24489,19 +24701,29 @@
       <c r="F35" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G35" s="5"/>
+      <c r="G35" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="1" t="str">
         <f aca="false">CONCATENATE(IF(I35="n","1","0"),IF(H35="n","1","0"),IF(G35="n","1","0"),IF(F35="n","1","0"),IF(E35="n","1","0"),IF(D35="n","1","0"),IF(C35="n","1","0"),IF(B35="n","1","0"))</f>
-        <v>00011100</v>
+        <v>00111100</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L35" s="1" t="str">
         <f aca="false">CONCATENATE("&amp;B",J35)</f>
-        <v>&amp;B00011100</v>
+        <v>&amp;B00111100</v>
+      </c>
+      <c r="M35" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B35="n","1","0"),IF(C35="n","1","0"),IF(D35="n","1","0"),IF(E35="n","1","0"),IF(F35="n","1","0"),IF(G35="n","1","0"),IF(H35="n","1","0"),IF(I35="n","1","0"))</f>
+        <v>00111100</v>
+      </c>
+      <c r="N35" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M35,",")</f>
+        <v>0B00111100,</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24515,21 +24737,27 @@
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
-      <c r="G36" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
       <c r="J36" s="1" t="str">
         <f aca="false">CONCATENATE(IF(I36="n","1","0"),IF(H36="n","1","0"),IF(G36="n","1","0"),IF(F36="n","1","0"),IF(E36="n","1","0"),IF(D36="n","1","0"),IF(C36="n","1","0"),IF(B36="n","1","0"))</f>
-        <v>00100100</v>
+        <v>00000100</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L36" s="1" t="str">
         <f aca="false">CONCATENATE("&amp;B",J36)</f>
-        <v>&amp;B00100100</v>
+        <v>&amp;B00000100</v>
+      </c>
+      <c r="M36" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B36="n","1","0"),IF(C36="n","1","0"),IF(D36="n","1","0"),IF(E36="n","1","0"),IF(F36="n","1","0"),IF(G36="n","1","0"),IF(H36="n","1","0"),IF(I36="n","1","0"))</f>
+        <v>00100000</v>
+      </c>
+      <c r="N36" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M36,",")</f>
+        <v>0B00100000,</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24569,6 +24797,14 @@
         <f aca="false">CONCATENATE("&amp;B",J37)</f>
         <v>&amp;B01111111</v>
       </c>
+      <c r="M37" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B37="n","1","0"),IF(C37="n","1","0"),IF(D37="n","1","0"),IF(E37="n","1","0"),IF(F37="n","1","0"),IF(G37="n","1","0"),IF(H37="n","1","0"),IF(I37="n","1","0"))</f>
+        <v>11111110</v>
+      </c>
+      <c r="N37" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M37,",")</f>
+        <v>0B11111110,</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="n">
@@ -24606,6 +24842,14 @@
       <c r="L38" s="1" t="str">
         <f aca="false">CONCATENATE("&amp;B",J38)</f>
         <v>&amp;B01111111</v>
+      </c>
+      <c r="M38" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B38="n","1","0"),IF(C38="n","1","0"),IF(D38="n","1","0"),IF(E38="n","1","0"),IF(F38="n","1","0"),IF(G38="n","1","0"),IF(H38="n","1","0"),IF(I38="n","1","0"))</f>
+        <v>11111110</v>
+      </c>
+      <c r="N38" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M38,",")</f>
+        <v>0B11111110,</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -24633,6 +24877,17 @@
         <f aca="false">CONCATENATE("&amp;B",J39)</f>
         <v>&amp;B00000100</v>
       </c>
+      <c r="M39" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B39="n","1","0"),IF(C39="n","1","0"),IF(D39="n","1","0"),IF(E39="n","1","0"),IF(F39="n","1","0"),IF(G39="n","1","0"),IF(H39="n","1","0"),IF(I39="n","1","0"))</f>
+        <v>00100000</v>
+      </c>
+      <c r="N39" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M39,",")</f>
+        <v>0B00100000,</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="1" t="n">
@@ -24662,6 +24917,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="n">
@@ -24696,6 +24952,14 @@
         <f aca="false">CONCATENATE("&amp;B",J42)</f>
         <v>&amp;B01111010</v>
       </c>
+      <c r="M42" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B42="n","1","0"),IF(C42="n","1","0"),IF(D42="n","1","0"),IF(E42="n","1","0"),IF(F42="n","1","0"),IF(G42="n","1","0"),IF(H42="n","1","0"),IF(I42="n","1","0"))</f>
+        <v>01011110</v>
+      </c>
+      <c r="N42" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M42,",")</f>
+        <v>0B01011110,</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="n">
@@ -24732,6 +24996,14 @@
         <f aca="false">CONCATENATE("&amp;B",J43)</f>
         <v>&amp;B01111011</v>
       </c>
+      <c r="M43" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B43="n","1","0"),IF(C43="n","1","0"),IF(D43="n","1","0"),IF(E43="n","1","0"),IF(F43="n","1","0"),IF(G43="n","1","0"),IF(H43="n","1","0"),IF(I43="n","1","0"))</f>
+        <v>11011110</v>
+      </c>
+      <c r="N43" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M43,",")</f>
+        <v>0B11011110,</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="n">
@@ -24762,6 +25034,14 @@
         <f aca="false">CONCATENATE("&amp;B",J44)</f>
         <v>&amp;B01001001</v>
       </c>
+      <c r="M44" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B44="n","1","0"),IF(C44="n","1","0"),IF(D44="n","1","0"),IF(E44="n","1","0"),IF(F44="n","1","0"),IF(G44="n","1","0"),IF(H44="n","1","0"),IF(I44="n","1","0"))</f>
+        <v>10010010</v>
+      </c>
+      <c r="N44" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M44,",")</f>
+        <v>0B10010010,</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="n">
@@ -24792,6 +25072,14 @@
         <f aca="false">CONCATENATE("&amp;B",J45)</f>
         <v>&amp;B01001001</v>
       </c>
+      <c r="M45" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B45="n","1","0"),IF(C45="n","1","0"),IF(D45="n","1","0"),IF(E45="n","1","0"),IF(F45="n","1","0"),IF(G45="n","1","0"),IF(H45="n","1","0"),IF(I45="n","1","0"))</f>
+        <v>10010010</v>
+      </c>
+      <c r="N45" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M45,",")</f>
+        <v>0B10010010,</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="n">
@@ -24826,6 +25114,14 @@
         <f aca="false">CONCATENATE("&amp;B",J46)</f>
         <v>&amp;B01001111</v>
       </c>
+      <c r="M46" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B46="n","1","0"),IF(C46="n","1","0"),IF(D46="n","1","0"),IF(E46="n","1","0"),IF(F46="n","1","0"),IF(G46="n","1","0"),IF(H46="n","1","0"),IF(I46="n","1","0"))</f>
+        <v>11110010</v>
+      </c>
+      <c r="N46" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M46,",")</f>
+        <v>0B11110010,</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="7" t="n">
@@ -24856,6 +25152,17 @@
         <f aca="false">CONCATENATE("&amp;B",J47)</f>
         <v>&amp;B01000110</v>
       </c>
+      <c r="M47" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B47="n","1","0"),IF(C47="n","1","0"),IF(D47="n","1","0"),IF(E47="n","1","0"),IF(F47="n","1","0"),IF(G47="n","1","0"),IF(H47="n","1","0"),IF(I47="n","1","0"))</f>
+        <v>01100010</v>
+      </c>
+      <c r="N47" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M47,",")</f>
+        <v>0B01100010,</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="1" t="n">
@@ -24885,6 +25192,7 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="n">
@@ -24919,6 +25227,14 @@
         <f aca="false">CONCATENATE("&amp;B",J50)</f>
         <v>&amp;B00111110</v>
       </c>
+      <c r="M50" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B50="n","1","0"),IF(C50="n","1","0"),IF(D50="n","1","0"),IF(E50="n","1","0"),IF(F50="n","1","0"),IF(G50="n","1","0"),IF(H50="n","1","0"),IF(I50="n","1","0"))</f>
+        <v>01111100</v>
+      </c>
+      <c r="N50" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M50,",")</f>
+        <v>0B01111100,</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="n">
@@ -24957,6 +25273,14 @@
         <f aca="false">CONCATENATE("&amp;B",J51)</f>
         <v>&amp;B01111111</v>
       </c>
+      <c r="M51" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B51="n","1","0"),IF(C51="n","1","0"),IF(D51="n","1","0"),IF(E51="n","1","0"),IF(F51="n","1","0"),IF(G51="n","1","0"),IF(H51="n","1","0"),IF(I51="n","1","0"))</f>
+        <v>11111110</v>
+      </c>
+      <c r="N51" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M51,",")</f>
+        <v>0B11111110,</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="n">
@@ -24987,6 +25311,14 @@
         <f aca="false">CONCATENATE("&amp;B",J52)</f>
         <v>&amp;B01001001</v>
       </c>
+      <c r="M52" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B52="n","1","0"),IF(C52="n","1","0"),IF(D52="n","1","0"),IF(E52="n","1","0"),IF(F52="n","1","0"),IF(G52="n","1","0"),IF(H52="n","1","0"),IF(I52="n","1","0"))</f>
+        <v>10010010</v>
+      </c>
+      <c r="N52" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M52,",")</f>
+        <v>0B10010010,</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="n">
@@ -25017,6 +25349,14 @@
         <f aca="false">CONCATENATE("&amp;B",J53)</f>
         <v>&amp;B01001001</v>
       </c>
+      <c r="M53" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B53="n","1","0"),IF(C53="n","1","0"),IF(D53="n","1","0"),IF(E53="n","1","0"),IF(F53="n","1","0"),IF(G53="n","1","0"),IF(H53="n","1","0"),IF(I53="n","1","0"))</f>
+        <v>10010010</v>
+      </c>
+      <c r="N53" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M53,",")</f>
+        <v>0B10010010,</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="n">
@@ -25036,18 +25376,28 @@
       </c>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
+      <c r="H54" s="5" t="s">
+        <v>0</v>
+      </c>
       <c r="I54" s="5"/>
       <c r="J54" s="1" t="str">
         <f aca="false">CONCATENATE(IF(I54="n","1","0"),IF(H54="n","1","0"),IF(G54="n","1","0"),IF(F54="n","1","0"),IF(E54="n","1","0"),IF(D54="n","1","0"),IF(C54="n","1","0"),IF(B54="n","1","0"))</f>
-        <v>00001111</v>
+        <v>01001111</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L54" s="1" t="str">
         <f aca="false">CONCATENATE("&amp;B",J54)</f>
-        <v>&amp;B00001111</v>
+        <v>&amp;B01001111</v>
+      </c>
+      <c r="M54" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B54="n","1","0"),IF(C54="n","1","0"),IF(D54="n","1","0"),IF(E54="n","1","0"),IF(F54="n","1","0"),IF(G54="n","1","0"),IF(H54="n","1","0"),IF(I54="n","1","0"))</f>
+        <v>11110010</v>
+      </c>
+      <c r="N54" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M54,",")</f>
+        <v>0B11110010,</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25077,6 +25427,17 @@
         <f aca="false">CONCATENATE("&amp;B",J55)</f>
         <v>&amp;B00000110</v>
       </c>
+      <c r="M55" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B55="n","1","0"),IF(C55="n","1","0"),IF(D55="n","1","0"),IF(E55="n","1","0"),IF(F55="n","1","0"),IF(G55="n","1","0"),IF(H55="n","1","0"),IF(I55="n","1","0"))</f>
+        <v>01100000</v>
+      </c>
+      <c r="N55" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M55,",")</f>
+        <v>0B01100000,</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M56" s="1"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="1" t="n">
@@ -25106,6 +25467,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="n">
@@ -25132,6 +25494,14 @@
         <f aca="false">CONCATENATE("&amp;B",J58)</f>
         <v>&amp;B01000000</v>
       </c>
+      <c r="M58" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B58="n","1","0"),IF(C58="n","1","0"),IF(D58="n","1","0"),IF(E58="n","1","0"),IF(F58="n","1","0"),IF(G58="n","1","0"),IF(H58="n","1","0"),IF(I58="n","1","0"))</f>
+        <v>00000010</v>
+      </c>
+      <c r="N58" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M58,",")</f>
+        <v>0B00000010,</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="n">
@@ -25164,6 +25534,14 @@
         <f aca="false">CONCATENATE("&amp;B",J59)</f>
         <v>&amp;B01000111</v>
       </c>
+      <c r="M59" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B59="n","1","0"),IF(C59="n","1","0"),IF(D59="n","1","0"),IF(E59="n","1","0"),IF(F59="n","1","0"),IF(G59="n","1","0"),IF(H59="n","1","0"),IF(I59="n","1","0"))</f>
+        <v>11100010</v>
+      </c>
+      <c r="N59" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M59,",")</f>
+        <v>0B11100010,</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="n">
@@ -25198,6 +25576,14 @@
         <f aca="false">CONCATENATE("&amp;B",J60)</f>
         <v>&amp;B01001111</v>
       </c>
+      <c r="M60" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B60="n","1","0"),IF(C60="n","1","0"),IF(D60="n","1","0"),IF(E60="n","1","0"),IF(F60="n","1","0"),IF(G60="n","1","0"),IF(H60="n","1","0"),IF(I60="n","1","0"))</f>
+        <v>11110010</v>
+      </c>
+      <c r="N60" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M60,",")</f>
+        <v>0B11110010,</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="n">
@@ -25227,6 +25613,14 @@
       <c r="L61" s="1" t="str">
         <f aca="false">CONCATENATE("&amp;B",J61)</f>
         <v>&amp;B01011000</v>
+      </c>
+      <c r="M61" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B61="n","1","0"),IF(C61="n","1","0"),IF(D61="n","1","0"),IF(E61="n","1","0"),IF(F61="n","1","0"),IF(G61="n","1","0"),IF(H61="n","1","0"),IF(I61="n","1","0"))</f>
+        <v>00011010</v>
+      </c>
+      <c r="N61" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M61,",")</f>
+        <v>0B00011010,</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25257,6 +25651,14 @@
       <c r="L62" s="1" t="str">
         <f aca="false">CONCATENATE("&amp;B",J62)</f>
         <v>&amp;B01110000</v>
+      </c>
+      <c r="M62" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B62="n","1","0"),IF(C62="n","1","0"),IF(D62="n","1","0"),IF(E62="n","1","0"),IF(F62="n","1","0"),IF(G62="n","1","0"),IF(H62="n","1","0"),IF(I62="n","1","0"))</f>
+        <v>00001110</v>
+      </c>
+      <c r="N62" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M62,",")</f>
+        <v>0B00001110,</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25286,6 +25688,17 @@
         <f aca="false">CONCATENATE("&amp;B",J63)</f>
         <v>&amp;B01100000</v>
       </c>
+      <c r="M63" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B63="n","1","0"),IF(C63="n","1","0"),IF(D63="n","1","0"),IF(E63="n","1","0"),IF(F63="n","1","0"),IF(G63="n","1","0"),IF(H63="n","1","0"),IF(I63="n","1","0"))</f>
+        <v>00000110</v>
+      </c>
+      <c r="N63" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M63,",")</f>
+        <v>0B00000110,</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M64" s="1"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="1" t="n">
@@ -25315,6 +25728,7 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="n">
@@ -25347,6 +25761,14 @@
         <f aca="false">CONCATENATE("&amp;B",J66)</f>
         <v>&amp;B00110110</v>
       </c>
+      <c r="M66" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B66="n","1","0"),IF(C66="n","1","0"),IF(D66="n","1","0"),IF(E66="n","1","0"),IF(F66="n","1","0"),IF(G66="n","1","0"),IF(H66="n","1","0"),IF(I66="n","1","0"))</f>
+        <v>01101100</v>
+      </c>
+      <c r="N66" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M66,",")</f>
+        <v>0B01101100,</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="n">
@@ -25385,6 +25807,14 @@
         <f aca="false">CONCATENATE("&amp;B",J67)</f>
         <v>&amp;B01111111</v>
       </c>
+      <c r="M67" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B67="n","1","0"),IF(C67="n","1","0"),IF(D67="n","1","0"),IF(E67="n","1","0"),IF(F67="n","1","0"),IF(G67="n","1","0"),IF(H67="n","1","0"),IF(I67="n","1","0"))</f>
+        <v>11111110</v>
+      </c>
+      <c r="N67" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M67,",")</f>
+        <v>0B11111110,</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4" t="n">
@@ -25415,6 +25845,14 @@
         <f aca="false">CONCATENATE("&amp;B",J68)</f>
         <v>&amp;B01001001</v>
       </c>
+      <c r="M68" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B68="n","1","0"),IF(C68="n","1","0"),IF(D68="n","1","0"),IF(E68="n","1","0"),IF(F68="n","1","0"),IF(G68="n","1","0"),IF(H68="n","1","0"),IF(I68="n","1","0"))</f>
+        <v>10010010</v>
+      </c>
+      <c r="N68" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M68,",")</f>
+        <v>0B10010010,</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="n">
@@ -25445,6 +25883,14 @@
         <f aca="false">CONCATENATE("&amp;B",J69)</f>
         <v>&amp;B01001001</v>
       </c>
+      <c r="M69" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B69="n","1","0"),IF(C69="n","1","0"),IF(D69="n","1","0"),IF(E69="n","1","0"),IF(F69="n","1","0"),IF(G69="n","1","0"),IF(H69="n","1","0"),IF(I69="n","1","0"))</f>
+        <v>10010010</v>
+      </c>
+      <c r="N69" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M69,",")</f>
+        <v>0B10010010,</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="n">
@@ -25482,6 +25928,14 @@
       <c r="L70" s="1" t="str">
         <f aca="false">CONCATENATE("&amp;B",J70)</f>
         <v>&amp;B01111111</v>
+      </c>
+      <c r="M70" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B70="n","1","0"),IF(C70="n","1","0"),IF(D70="n","1","0"),IF(E70="n","1","0"),IF(F70="n","1","0"),IF(G70="n","1","0"),IF(H70="n","1","0"),IF(I70="n","1","0"))</f>
+        <v>11111110</v>
+      </c>
+      <c r="N70" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M70,",")</f>
+        <v>0B11111110,</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25515,6 +25969,17 @@
         <f aca="false">CONCATENATE("&amp;B",J71)</f>
         <v>&amp;B00110110</v>
       </c>
+      <c r="M71" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B71="n","1","0"),IF(C71="n","1","0"),IF(D71="n","1","0"),IF(E71="n","1","0"),IF(F71="n","1","0"),IF(G71="n","1","0"),IF(H71="n","1","0"),IF(I71="n","1","0"))</f>
+        <v>01101100</v>
+      </c>
+      <c r="N71" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M71,",")</f>
+        <v>0B01101100,</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M72" s="1"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="1" t="n">
@@ -25544,6 +26009,7 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="4" t="n">
@@ -25572,6 +26038,14 @@
         <f aca="false">CONCATENATE("&amp;B",J74)</f>
         <v>&amp;B00110000</v>
       </c>
+      <c r="M74" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B74="n","1","0"),IF(C74="n","1","0"),IF(D74="n","1","0"),IF(E74="n","1","0"),IF(F74="n","1","0"),IF(G74="n","1","0"),IF(H74="n","1","0"),IF(I74="n","1","0"))</f>
+        <v>00001100</v>
+      </c>
+      <c r="N74" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M74,",")</f>
+        <v>0B00001100,</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="n">
@@ -25606,6 +26080,14 @@
         <f aca="false">CONCATENATE("&amp;B",J75)</f>
         <v>&amp;B01111001</v>
       </c>
+      <c r="M75" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B75="n","1","0"),IF(C75="n","1","0"),IF(D75="n","1","0"),IF(E75="n","1","0"),IF(F75="n","1","0"),IF(G75="n","1","0"),IF(H75="n","1","0"),IF(I75="n","1","0"))</f>
+        <v>10011110</v>
+      </c>
+      <c r="N75" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M75,",")</f>
+        <v>0B10011110,</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="4" t="n">
@@ -25636,6 +26118,14 @@
         <f aca="false">CONCATENATE("&amp;B",J76)</f>
         <v>&amp;B01001001</v>
       </c>
+      <c r="M76" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B76="n","1","0"),IF(C76="n","1","0"),IF(D76="n","1","0"),IF(E76="n","1","0"),IF(F76="n","1","0"),IF(G76="n","1","0"),IF(H76="n","1","0"),IF(I76="n","1","0"))</f>
+        <v>10010010</v>
+      </c>
+      <c r="N76" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M76,",")</f>
+        <v>0B10010010,</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="4" t="n">
@@ -25666,6 +26156,14 @@
         <f aca="false">CONCATENATE("&amp;B",J77)</f>
         <v>&amp;B01001001</v>
       </c>
+      <c r="M77" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B77="n","1","0"),IF(C77="n","1","0"),IF(D77="n","1","0"),IF(E77="n","1","0"),IF(F77="n","1","0"),IF(G77="n","1","0"),IF(H77="n","1","0"),IF(I77="n","1","0"))</f>
+        <v>10010010</v>
+      </c>
+      <c r="N77" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M77,",")</f>
+        <v>0B10010010,</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="4" t="n">
@@ -25703,6 +26201,14 @@
       <c r="L78" s="1" t="str">
         <f aca="false">CONCATENATE("&amp;B",J78)</f>
         <v>&amp;B01111111</v>
+      </c>
+      <c r="M78" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B78="n","1","0"),IF(C78="n","1","0"),IF(D78="n","1","0"),IF(E78="n","1","0"),IF(F78="n","1","0"),IF(G78="n","1","0"),IF(H78="n","1","0"),IF(I78="n","1","0"))</f>
+        <v>11111110</v>
+      </c>
+      <c r="N78" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M78,",")</f>
+        <v>0B11111110,</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25738,6 +26244,17 @@
         <f aca="false">CONCATENATE("&amp;B",J79)</f>
         <v>&amp;B00111110</v>
       </c>
+      <c r="M79" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B79="n","1","0"),IF(C79="n","1","0"),IF(D79="n","1","0"),IF(E79="n","1","0"),IF(F79="n","1","0"),IF(G79="n","1","0"),IF(H79="n","1","0"),IF(I79="n","1","0"))</f>
+        <v>01111100</v>
+      </c>
+      <c r="N79" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M79,",")</f>
+        <v>0B01111100,</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M80" s="1"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B81" s="1" t="n">
@@ -25767,6 +26284,7 @@
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
+      <c r="M81" s="1"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="4" t="n">
@@ -25791,6 +26309,14 @@
         <f aca="false">CONCATENATE("&amp;B",J82)</f>
         <v>&amp;B00000000</v>
       </c>
+      <c r="M82" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B82="n","1","0"),IF(C82="n","1","0"),IF(D82="n","1","0"),IF(E82="n","1","0"),IF(F82="n","1","0"),IF(G82="n","1","0"),IF(H82="n","1","0"),IF(I82="n","1","0"))</f>
+        <v>00000000</v>
+      </c>
+      <c r="N82" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M82,",")</f>
+        <v>0B00000000,</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="4" t="n">
@@ -25815,6 +26341,14 @@
         <f aca="false">CONCATENATE("&amp;B",J83)</f>
         <v>&amp;B00000000</v>
       </c>
+      <c r="M83" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B83="n","1","0"),IF(C83="n","1","0"),IF(D83="n","1","0"),IF(E83="n","1","0"),IF(F83="n","1","0"),IF(G83="n","1","0"),IF(H83="n","1","0"),IF(I83="n","1","0"))</f>
+        <v>00000000</v>
+      </c>
+      <c r="N83" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M83,",")</f>
+        <v>0B00000000,</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="4" t="n">
@@ -25839,6 +26373,14 @@
         <f aca="false">CONCATENATE("&amp;B",J84)</f>
         <v>&amp;B00000000</v>
       </c>
+      <c r="M84" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B84="n","1","0"),IF(C84="n","1","0"),IF(D84="n","1","0"),IF(E84="n","1","0"),IF(F84="n","1","0"),IF(G84="n","1","0"),IF(H84="n","1","0"),IF(I84="n","1","0"))</f>
+        <v>00000000</v>
+      </c>
+      <c r="N84" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M84,",")</f>
+        <v>0B00000000,</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="n">
@@ -25863,6 +26405,14 @@
         <f aca="false">CONCATENATE("&amp;B",J85)</f>
         <v>&amp;B00000000</v>
       </c>
+      <c r="M85" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B85="n","1","0"),IF(C85="n","1","0"),IF(D85="n","1","0"),IF(E85="n","1","0"),IF(F85="n","1","0"),IF(G85="n","1","0"),IF(H85="n","1","0"),IF(I85="n","1","0"))</f>
+        <v>00000000</v>
+      </c>
+      <c r="N85" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M85,",")</f>
+        <v>0B00000000,</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="4" t="n">
@@ -25887,6 +26437,14 @@
         <f aca="false">CONCATENATE("&amp;B",J86)</f>
         <v>&amp;B00000000</v>
       </c>
+      <c r="M86" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B86="n","1","0"),IF(C86="n","1","0"),IF(D86="n","1","0"),IF(E86="n","1","0"),IF(F86="n","1","0"),IF(G86="n","1","0"),IF(H86="n","1","0"),IF(I86="n","1","0"))</f>
+        <v>00000000</v>
+      </c>
+      <c r="N86" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M86,",")</f>
+        <v>0B00000000,</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="7" t="n">
@@ -25911,6 +26469,14 @@
         <f aca="false">CONCATENATE("&amp;B",J87)</f>
         <v>&amp;B00000000</v>
       </c>
+      <c r="M87" s="1" t="str">
+        <f aca="false">CONCATENATE(IF(B87="n","1","0"),IF(C87="n","1","0"),IF(D87="n","1","0"),IF(E87="n","1","0"),IF(F87="n","1","0"),IF(G87="n","1","0"),IF(H87="n","1","0"),IF(I87="n","1","0"))</f>
+        <v>00000000</v>
+      </c>
+      <c r="N87" s="0" t="str">
+        <f aca="false">CONCATENATE("0B",M87,",")</f>
+        <v>0B00000000,</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>